<commit_message>
update vaccine number until 2021/12/31
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccination_number.xlsx
+++ b/data/vaccine/vaccination_number.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjlee/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyunjeong/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4947CF00-97C8-824F-898F-3848F863EEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A70C423-ED63-324F-8E03-8DF9EE8E2633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="580" windowWidth="15140" windowHeight="13380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13120" yWindow="1380" windowWidth="13180" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="212">
   <si>
     <t>2021.03.07</t>
   </si>
@@ -639,17 +639,62 @@
   </si>
   <si>
     <t>2021.02.23</t>
+  </si>
+  <si>
+    <t>2021.09.01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021.09.02</t>
+  </si>
+  <si>
+    <t>2021.09.03</t>
+  </si>
+  <si>
+    <t>2021.09.04</t>
+  </si>
+  <si>
+    <t>2021.09.05</t>
+  </si>
+  <si>
+    <t>2021.09.06</t>
+  </si>
+  <si>
+    <t>2021.09.07</t>
+  </si>
+  <si>
+    <t>2021.09.08</t>
+  </si>
+  <si>
+    <t>2021.09.09</t>
+  </si>
+  <si>
+    <t>09/02-09/09</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -674,7 +719,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -683,6 +728,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -868,7 +922,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Normal Style 1 - Accent 1" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Normal Style 1 - Accent 1" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="13"/>
       <tableStyleElement type="headerRow" dxfId="12"/>
       <tableStyleElement type="totalRow" dxfId="11"/>
@@ -877,7 +931,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="8"/>
       <tableStyleElement type="firstColumnStripe" dxfId="7"/>
     </tableStyle>
-    <tableStyle name="Light Style 1 - Accent 1" table="0" count="8" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Light Style 1 - Accent 1" table="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -1191,10 +1245,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C321"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="C199" sqref="C199"/>
+    <sheetView tabSelected="1" topLeftCell="A300" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="D312" sqref="D312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -1211,8 +1265,8 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>199</v>
+      <c r="A2" s="5">
+        <v>44242</v>
       </c>
       <c r="B2" s="2">
         <f>서울!B2+경기!B2</f>
@@ -1224,8 +1278,8 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>198</v>
+      <c r="A3" s="5">
+        <v>44243</v>
       </c>
       <c r="B3" s="2">
         <f>서울!B3+경기!B3</f>
@@ -1237,8 +1291,8 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>191</v>
+      <c r="A4" s="5">
+        <v>44244</v>
       </c>
       <c r="B4" s="2">
         <f>서울!B4+경기!B4</f>
@@ -1250,8 +1304,8 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>190</v>
+      <c r="A5" s="5">
+        <v>44245</v>
       </c>
       <c r="B5" s="2">
         <f>서울!B5+경기!B5</f>
@@ -1263,8 +1317,8 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>189</v>
+      <c r="A6" s="5">
+        <v>44246</v>
       </c>
       <c r="B6" s="2">
         <f>서울!B6+경기!B6</f>
@@ -1276,8 +1330,8 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>193</v>
+      <c r="A7" s="5">
+        <v>44247</v>
       </c>
       <c r="B7" s="2">
         <f>서울!B7+경기!B7</f>
@@ -1289,8 +1343,8 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>192</v>
+      <c r="A8" s="5">
+        <v>44248</v>
       </c>
       <c r="B8" s="2">
         <f>서울!B8+경기!B8</f>
@@ -1302,8 +1356,8 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>188</v>
+      <c r="A9" s="5">
+        <v>44249</v>
       </c>
       <c r="B9" s="2">
         <f>서울!B9+경기!B9</f>
@@ -1315,8 +1369,8 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>201</v>
+      <c r="A10" s="5">
+        <v>44250</v>
       </c>
       <c r="B10" s="2">
         <f>서울!B10+경기!B10</f>
@@ -1328,8 +1382,8 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>200</v>
+      <c r="A11" s="5">
+        <v>44251</v>
       </c>
       <c r="B11" s="2">
         <f>서울!B11+경기!B11</f>
@@ -1341,8 +1395,8 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>196</v>
+      <c r="A12" s="5">
+        <v>44252</v>
       </c>
       <c r="B12" s="2">
         <f>서울!B12+경기!B12</f>
@@ -1354,8 +1408,8 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>11</v>
+      <c r="A13" s="5">
+        <v>44253</v>
       </c>
       <c r="B13" s="2">
         <f>서울!B13+경기!B13</f>
@@ -1367,8 +1421,8 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>3</v>
+      <c r="A14" s="5">
+        <v>44254</v>
       </c>
       <c r="B14" s="2">
         <f>서울!B14+경기!B14</f>
@@ -1380,8 +1434,8 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>4</v>
+      <c r="A15" s="5">
+        <v>44255</v>
       </c>
       <c r="B15" s="2">
         <f>서울!B15+경기!B15</f>
@@ -1393,8 +1447,8 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>2</v>
+      <c r="A16" s="5">
+        <v>44256</v>
       </c>
       <c r="B16" s="2">
         <f>서울!B16+경기!B16</f>
@@ -1406,8 +1460,8 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>1</v>
+      <c r="A17" s="5">
+        <v>44257</v>
       </c>
       <c r="B17" s="2">
         <f>서울!B17+경기!B17</f>
@@ -1419,8 +1473,8 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>7</v>
+      <c r="A18" s="5">
+        <v>44258</v>
       </c>
       <c r="B18" s="2">
         <f>서울!B18+경기!B18</f>
@@ -1432,8 +1486,8 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>6</v>
+      <c r="A19" s="5">
+        <v>44259</v>
       </c>
       <c r="B19" s="2">
         <f>서울!B19+경기!B19</f>
@@ -1445,8 +1499,8 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>8</v>
+      <c r="A20" s="5">
+        <v>44260</v>
       </c>
       <c r="B20" s="2">
         <f>서울!B20+경기!B20</f>
@@ -1458,8 +1512,8 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>9</v>
+      <c r="A21" s="5">
+        <v>44261</v>
       </c>
       <c r="B21" s="2">
         <f>서울!B21+경기!B21</f>
@@ -1471,8 +1525,8 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>0</v>
+      <c r="A22" s="5">
+        <v>44262</v>
       </c>
       <c r="B22" s="2">
         <f>서울!B22+경기!B22</f>
@@ -1484,8 +1538,8 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>5</v>
+      <c r="A23" s="5">
+        <v>44263</v>
       </c>
       <c r="B23" s="2">
         <f>서울!B23+경기!B23</f>
@@ -1497,8 +1551,8 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>43</v>
+      <c r="A24" s="5">
+        <v>44264</v>
       </c>
       <c r="B24" s="2">
         <f>서울!B24+경기!B24</f>
@@ -1510,8 +1564,8 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>42</v>
+      <c r="A25" s="5">
+        <v>44265</v>
       </c>
       <c r="B25" s="2">
         <f>서울!B25+경기!B25</f>
@@ -1523,8 +1577,8 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>41</v>
+      <c r="A26" s="5">
+        <v>44266</v>
       </c>
       <c r="B26" s="2">
         <f>서울!B26+경기!B26</f>
@@ -1536,8 +1590,8 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>44</v>
+      <c r="A27" s="5">
+        <v>44267</v>
       </c>
       <c r="B27" s="2">
         <f>서울!B27+경기!B27</f>
@@ -1549,8 +1603,8 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>46</v>
+      <c r="A28" s="5">
+        <v>44268</v>
       </c>
       <c r="B28" s="2">
         <f>서울!B28+경기!B28</f>
@@ -1562,8 +1616,8 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>47</v>
+      <c r="A29" s="5">
+        <v>44269</v>
       </c>
       <c r="B29" s="2">
         <f>서울!B29+경기!B29</f>
@@ -1575,8 +1629,8 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>45</v>
+      <c r="A30" s="5">
+        <v>44270</v>
       </c>
       <c r="B30" s="2">
         <f>서울!B30+경기!B30</f>
@@ -1588,8 +1642,8 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>49</v>
+      <c r="A31" s="5">
+        <v>44271</v>
       </c>
       <c r="B31" s="2">
         <f>서울!B31+경기!B31</f>
@@ -1601,8 +1655,8 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>48</v>
+      <c r="A32" s="5">
+        <v>44272</v>
       </c>
       <c r="B32" s="2">
         <f>서울!B32+경기!B32</f>
@@ -1614,8 +1668,8 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>50</v>
+      <c r="A33" s="5">
+        <v>44273</v>
       </c>
       <c r="B33" s="2">
         <f>서울!B33+경기!B33</f>
@@ -1627,8 +1681,8 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>53</v>
+      <c r="A34" s="5">
+        <v>44274</v>
       </c>
       <c r="B34" s="2">
         <f>서울!B34+경기!B34</f>
@@ -1640,8 +1694,8 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>52</v>
+      <c r="A35" s="5">
+        <v>44275</v>
       </c>
       <c r="B35" s="2">
         <f>서울!B35+경기!B35</f>
@@ -1653,8 +1707,8 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>54</v>
+      <c r="A36" s="5">
+        <v>44276</v>
       </c>
       <c r="B36" s="2">
         <f>서울!B36+경기!B36</f>
@@ -1666,8 +1720,8 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>51</v>
+      <c r="A37" s="5">
+        <v>44277</v>
       </c>
       <c r="B37" s="2">
         <f>서울!B37+경기!B37</f>
@@ -1679,8 +1733,8 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>56</v>
+      <c r="A38" s="5">
+        <v>44278</v>
       </c>
       <c r="B38" s="2">
         <f>서울!B38+경기!B38</f>
@@ -1692,8 +1746,8 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>55</v>
+      <c r="A39" s="5">
+        <v>44279</v>
       </c>
       <c r="B39" s="2">
         <f>서울!B39+경기!B39</f>
@@ -1705,8 +1759,8 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>57</v>
+      <c r="A40" s="5">
+        <v>44280</v>
       </c>
       <c r="B40" s="2">
         <f>서울!B40+경기!B40</f>
@@ -1718,8 +1772,8 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>60</v>
+      <c r="A41" s="5">
+        <v>44281</v>
       </c>
       <c r="B41" s="2">
         <f>서울!B41+경기!B41</f>
@@ -1731,8 +1785,8 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>59</v>
+      <c r="A42" s="5">
+        <v>44282</v>
       </c>
       <c r="B42" s="2">
         <f>서울!B42+경기!B42</f>
@@ -1744,8 +1798,8 @@
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>58</v>
+      <c r="A43" s="5">
+        <v>44283</v>
       </c>
       <c r="B43" s="2">
         <f>서울!B43+경기!B43</f>
@@ -1757,8 +1811,8 @@
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>63</v>
+      <c r="A44" s="5">
+        <v>44284</v>
       </c>
       <c r="B44" s="2">
         <f>서울!B44+경기!B44</f>
@@ -1770,8 +1824,8 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>61</v>
+      <c r="A45" s="5">
+        <v>44285</v>
       </c>
       <c r="B45" s="2">
         <f>서울!B45+경기!B45</f>
@@ -1783,8 +1837,8 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>62</v>
+      <c r="A46" s="5">
+        <v>44286</v>
       </c>
       <c r="B46" s="2">
         <f>서울!B46+경기!B46</f>
@@ -1796,8 +1850,8 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>65</v>
+      <c r="A47" s="5">
+        <v>44287</v>
       </c>
       <c r="B47" s="2">
         <f>서울!B47+경기!B47</f>
@@ -1809,8 +1863,8 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>66</v>
+      <c r="A48" s="5">
+        <v>44288</v>
       </c>
       <c r="B48" s="2">
         <f>서울!B48+경기!B48</f>
@@ -1822,8 +1876,8 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>64</v>
+      <c r="A49" s="5">
+        <v>44289</v>
       </c>
       <c r="B49" s="2">
         <f>서울!B49+경기!B49</f>
@@ -1835,8 +1889,8 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>67</v>
+      <c r="A50" s="5">
+        <v>44290</v>
       </c>
       <c r="B50" s="2">
         <f>서울!B50+경기!B50</f>
@@ -1848,8 +1902,8 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>69</v>
+      <c r="A51" s="5">
+        <v>44291</v>
       </c>
       <c r="B51" s="2">
         <f>서울!B51+경기!B51</f>
@@ -1861,8 +1915,8 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>68</v>
+      <c r="A52" s="5">
+        <v>44292</v>
       </c>
       <c r="B52" s="2">
         <f>서울!B52+경기!B52</f>
@@ -1874,8 +1928,8 @@
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>70</v>
+      <c r="A53" s="5">
+        <v>44293</v>
       </c>
       <c r="B53" s="2">
         <f>서울!B53+경기!B53</f>
@@ -1887,8 +1941,8 @@
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>71</v>
+      <c r="A54" s="5">
+        <v>44294</v>
       </c>
       <c r="B54" s="2">
         <f>서울!B54+경기!B54</f>
@@ -1900,8 +1954,8 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>72</v>
+      <c r="A55" s="5">
+        <v>44295</v>
       </c>
       <c r="B55" s="2">
         <f>서울!B55+경기!B55</f>
@@ -1913,8 +1967,8 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>76</v>
+      <c r="A56" s="5">
+        <v>44296</v>
       </c>
       <c r="B56" s="2">
         <f>서울!B56+경기!B56</f>
@@ -1926,8 +1980,8 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>74</v>
+      <c r="A57" s="5">
+        <v>44297</v>
       </c>
       <c r="B57" s="2">
         <f>서울!B57+경기!B57</f>
@@ -1939,8 +1993,8 @@
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>73</v>
+      <c r="A58" s="5">
+        <v>44298</v>
       </c>
       <c r="B58" s="2">
         <f>서울!B58+경기!B58</f>
@@ -1952,8 +2006,8 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>75</v>
+      <c r="A59" s="5">
+        <v>44299</v>
       </c>
       <c r="B59" s="2">
         <f>서울!B59+경기!B59</f>
@@ -1965,8 +2019,8 @@
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>78</v>
+      <c r="A60" s="5">
+        <v>44300</v>
       </c>
       <c r="B60" s="2">
         <f>서울!B60+경기!B60</f>
@@ -1978,8 +2032,8 @@
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>79</v>
+      <c r="A61" s="5">
+        <v>44301</v>
       </c>
       <c r="B61" s="2">
         <f>서울!B61+경기!B61</f>
@@ -1991,8 +2045,8 @@
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>77</v>
+      <c r="A62" s="5">
+        <v>44302</v>
       </c>
       <c r="B62" s="2">
         <f>서울!B62+경기!B62</f>
@@ -2004,8 +2058,8 @@
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>81</v>
+      <c r="A63" s="5">
+        <v>44303</v>
       </c>
       <c r="B63" s="2">
         <f>서울!B63+경기!B63</f>
@@ -2017,8 +2071,8 @@
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>80</v>
+      <c r="A64" s="5">
+        <v>44304</v>
       </c>
       <c r="B64" s="2">
         <f>서울!B64+경기!B64</f>
@@ -2030,8 +2084,8 @@
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>82</v>
+      <c r="A65" s="5">
+        <v>44305</v>
       </c>
       <c r="B65" s="2">
         <f>서울!B65+경기!B65</f>
@@ -2043,8 +2097,8 @@
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>35</v>
+      <c r="A66" s="5">
+        <v>44306</v>
       </c>
       <c r="B66" s="2">
         <f>서울!B66+경기!B66</f>
@@ -2056,8 +2110,8 @@
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>33</v>
+      <c r="A67" s="5">
+        <v>44307</v>
       </c>
       <c r="B67" s="2">
         <f>서울!B67+경기!B67</f>
@@ -2069,8 +2123,8 @@
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" t="s">
-        <v>34</v>
+      <c r="A68" s="5">
+        <v>44308</v>
       </c>
       <c r="B68" s="2">
         <f>서울!B68+경기!B68</f>
@@ -2082,8 +2136,8 @@
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" t="s">
-        <v>37</v>
+      <c r="A69" s="5">
+        <v>44309</v>
       </c>
       <c r="B69" s="2">
         <f>서울!B69+경기!B69</f>
@@ -2095,8 +2149,8 @@
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" t="s">
-        <v>38</v>
+      <c r="A70" s="5">
+        <v>44310</v>
       </c>
       <c r="B70" s="2">
         <f>서울!B70+경기!B70</f>
@@ -2108,8 +2162,8 @@
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>36</v>
+      <c r="A71" s="5">
+        <v>44311</v>
       </c>
       <c r="B71" s="2">
         <f>서울!B71+경기!B71</f>
@@ -2121,8 +2175,8 @@
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>40</v>
+      <c r="A72" s="5">
+        <v>44312</v>
       </c>
       <c r="B72" s="2">
         <f>서울!B72+경기!B72</f>
@@ -2134,8 +2188,8 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>39</v>
+      <c r="A73" s="5">
+        <v>44313</v>
       </c>
       <c r="B73" s="2">
         <f>서울!B73+경기!B73</f>
@@ -2147,8 +2201,8 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>92</v>
+      <c r="A74" s="5">
+        <v>44314</v>
       </c>
       <c r="B74" s="2">
         <f>서울!B74+경기!B74</f>
@@ -2160,8 +2214,8 @@
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>93</v>
+      <c r="A75" s="5">
+        <v>44315</v>
       </c>
       <c r="B75" s="2">
         <f>서울!B75+경기!B75</f>
@@ -2173,8 +2227,8 @@
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>91</v>
+      <c r="A76" s="5">
+        <v>44316</v>
       </c>
       <c r="B76" s="2">
         <f>서울!B76+경기!B76</f>
@@ -2186,8 +2240,8 @@
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>95</v>
+      <c r="A77" s="5">
+        <v>44317</v>
       </c>
       <c r="B77" s="2">
         <f>서울!B77+경기!B77</f>
@@ -2199,8 +2253,8 @@
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>96</v>
+      <c r="A78" s="5">
+        <v>44318</v>
       </c>
       <c r="B78" s="2">
         <f>서울!B78+경기!B78</f>
@@ -2212,8 +2266,8 @@
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>94</v>
+      <c r="A79" s="5">
+        <v>44319</v>
       </c>
       <c r="B79" s="2">
         <f>서울!B79+경기!B79</f>
@@ -2225,8 +2279,8 @@
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>98</v>
+      <c r="A80" s="5">
+        <v>44320</v>
       </c>
       <c r="B80" s="2">
         <f>서울!B80+경기!B80</f>
@@ -2238,8 +2292,8 @@
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>97</v>
+      <c r="A81" s="5">
+        <v>44321</v>
       </c>
       <c r="B81" s="2">
         <f>서울!B81+경기!B81</f>
@@ -2251,8 +2305,8 @@
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>101</v>
+      <c r="A82" s="5">
+        <v>44322</v>
       </c>
       <c r="B82" s="2">
         <f>서울!B82+경기!B82</f>
@@ -2264,8 +2318,8 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>100</v>
+      <c r="A83" s="5">
+        <v>44323</v>
       </c>
       <c r="B83" s="2">
         <f>서울!B83+경기!B83</f>
@@ -2277,8 +2331,8 @@
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" t="s">
-        <v>99</v>
+      <c r="A84" s="5">
+        <v>44324</v>
       </c>
       <c r="B84" s="2">
         <f>서울!B84+경기!B84</f>
@@ -2290,8 +2344,8 @@
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" t="s">
-        <v>103</v>
+      <c r="A85" s="5">
+        <v>44325</v>
       </c>
       <c r="B85" s="2">
         <f>서울!B85+경기!B85</f>
@@ -2303,8 +2357,8 @@
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" t="s">
-        <v>102</v>
+      <c r="A86" s="5">
+        <v>44326</v>
       </c>
       <c r="B86" s="2">
         <f>서울!B86+경기!B86</f>
@@ -2316,8 +2370,8 @@
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" t="s">
-        <v>106</v>
+      <c r="A87" s="5">
+        <v>44327</v>
       </c>
       <c r="B87" s="2">
         <f>서울!B87+경기!B87</f>
@@ -2329,8 +2383,8 @@
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>105</v>
+      <c r="A88" s="5">
+        <v>44328</v>
       </c>
       <c r="B88" s="2">
         <f>서울!B88+경기!B88</f>
@@ -2342,8 +2396,8 @@
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" t="s">
-        <v>104</v>
+      <c r="A89" s="5">
+        <v>44329</v>
       </c>
       <c r="B89" s="2">
         <f>서울!B89+경기!B89</f>
@@ -2355,8 +2409,8 @@
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" t="s">
-        <v>107</v>
+      <c r="A90" s="5">
+        <v>44330</v>
       </c>
       <c r="B90" s="2">
         <f>서울!B90+경기!B90</f>
@@ -2368,8 +2422,8 @@
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" t="s">
-        <v>108</v>
+      <c r="A91" s="5">
+        <v>44331</v>
       </c>
       <c r="B91" s="2">
         <f>서울!B91+경기!B91</f>
@@ -2381,8 +2435,8 @@
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>111</v>
+      <c r="A92" s="5">
+        <v>44332</v>
       </c>
       <c r="B92" s="2">
         <f>서울!B92+경기!B92</f>
@@ -2394,8 +2448,8 @@
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" t="s">
-        <v>110</v>
+      <c r="A93" s="5">
+        <v>44333</v>
       </c>
       <c r="B93" s="2">
         <f>서울!B93+경기!B93</f>
@@ -2407,8 +2461,8 @@
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" t="s">
-        <v>109</v>
+      <c r="A94" s="5">
+        <v>44334</v>
       </c>
       <c r="B94" s="2">
         <f>서울!B94+경기!B94</f>
@@ -2420,8 +2474,8 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>114</v>
+      <c r="A95" s="5">
+        <v>44335</v>
       </c>
       <c r="B95" s="2">
         <f>서울!B95+경기!B95</f>
@@ -2433,8 +2487,8 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" t="s">
-        <v>113</v>
+      <c r="A96" s="5">
+        <v>44336</v>
       </c>
       <c r="B96" s="2">
         <f>서울!B96+경기!B96</f>
@@ -2446,8 +2500,8 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" t="s">
-        <v>112</v>
+      <c r="A97" s="5">
+        <v>44337</v>
       </c>
       <c r="B97" s="2">
         <f>서울!B97+경기!B97</f>
@@ -2459,8 +2513,8 @@
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>115</v>
+      <c r="A98" s="5">
+        <v>44338</v>
       </c>
       <c r="B98" s="2">
         <f>서울!B98+경기!B98</f>
@@ -2472,8 +2526,8 @@
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" t="s">
-        <v>117</v>
+      <c r="A99" s="5">
+        <v>44339</v>
       </c>
       <c r="B99" s="2">
         <f>서울!B99+경기!B99</f>
@@ -2485,8 +2539,8 @@
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>116</v>
+      <c r="A100" s="5">
+        <v>44340</v>
       </c>
       <c r="B100" s="2">
         <f>서울!B100+경기!B100</f>
@@ -2498,8 +2552,8 @@
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>118</v>
+      <c r="A101" s="5">
+        <v>44341</v>
       </c>
       <c r="B101" s="2">
         <f>서울!B101+경기!B101</f>
@@ -2511,8 +2565,8 @@
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" t="s">
-        <v>119</v>
+      <c r="A102" s="5">
+        <v>44342</v>
       </c>
       <c r="B102" s="2">
         <f>서울!B102+경기!B102</f>
@@ -2524,8 +2578,8 @@
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" t="s">
-        <v>121</v>
+      <c r="A103" s="5">
+        <v>44343</v>
       </c>
       <c r="B103" s="2">
         <f>서울!B103+경기!B103</f>
@@ -2537,8 +2591,8 @@
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" t="s">
-        <v>120</v>
+      <c r="A104" s="5">
+        <v>44344</v>
       </c>
       <c r="B104" s="2">
         <f>서울!B104+경기!B104</f>
@@ -2550,8 +2604,8 @@
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" t="s">
-        <v>123</v>
+      <c r="A105" s="5">
+        <v>44345</v>
       </c>
       <c r="B105" s="2">
         <f>서울!B105+경기!B105</f>
@@ -2563,8 +2617,8 @@
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>124</v>
+      <c r="A106" s="5">
+        <v>44346</v>
       </c>
       <c r="B106" s="2">
         <f>서울!B106+경기!B106</f>
@@ -2576,8 +2630,8 @@
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>122</v>
+      <c r="A107" s="5">
+        <v>44347</v>
       </c>
       <c r="B107" s="2">
         <f>서울!B107+경기!B107</f>
@@ -2589,8 +2643,8 @@
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>85</v>
+      <c r="A108" s="5">
+        <v>44348</v>
       </c>
       <c r="B108" s="2">
         <f>서울!B108+경기!B108</f>
@@ -2602,8 +2656,8 @@
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" t="s">
-        <v>83</v>
+      <c r="A109" s="5">
+        <v>44349</v>
       </c>
       <c r="B109" s="2">
         <f>서울!B109+경기!B109</f>
@@ -2615,8 +2669,8 @@
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" t="s">
-        <v>84</v>
+      <c r="A110" s="5">
+        <v>44350</v>
       </c>
       <c r="B110" s="2">
         <f>서울!B110+경기!B110</f>
@@ -2628,8 +2682,8 @@
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" t="s">
-        <v>86</v>
+      <c r="A111" s="5">
+        <v>44351</v>
       </c>
       <c r="B111" s="2">
         <f>서울!B111+경기!B111</f>
@@ -2641,8 +2695,8 @@
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" t="s">
-        <v>87</v>
+      <c r="A112" s="5">
+        <v>44352</v>
       </c>
       <c r="B112" s="2">
         <f>서울!B112+경기!B112</f>
@@ -2654,8 +2708,8 @@
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" t="s">
-        <v>89</v>
+      <c r="A113" s="5">
+        <v>44353</v>
       </c>
       <c r="B113" s="2">
         <f>서울!B113+경기!B113</f>
@@ -2667,8 +2721,8 @@
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" t="s">
-        <v>90</v>
+      <c r="A114" s="5">
+        <v>44354</v>
       </c>
       <c r="B114" s="2">
         <f>서울!B114+경기!B114</f>
@@ -2680,8 +2734,8 @@
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" t="s">
-        <v>88</v>
+      <c r="A115" s="5">
+        <v>44355</v>
       </c>
       <c r="B115" s="2">
         <f>서울!B115+경기!B115</f>
@@ -2693,8 +2747,8 @@
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" t="s">
-        <v>22</v>
+      <c r="A116" s="5">
+        <v>44356</v>
       </c>
       <c r="B116" s="2">
         <f>서울!B116+경기!B116</f>
@@ -2706,8 +2760,8 @@
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" t="s">
-        <v>20</v>
+      <c r="A117" s="5">
+        <v>44357</v>
       </c>
       <c r="B117" s="2">
         <f>서울!B117+경기!B117</f>
@@ -2719,8 +2773,8 @@
       </c>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" t="s">
-        <v>21</v>
+      <c r="A118" s="5">
+        <v>44358</v>
       </c>
       <c r="B118" s="2">
         <f>서울!B118+경기!B118</f>
@@ -2732,8 +2786,8 @@
       </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" t="s">
-        <v>24</v>
+      <c r="A119" s="5">
+        <v>44359</v>
       </c>
       <c r="B119" s="2">
         <f>서울!B119+경기!B119</f>
@@ -2745,8 +2799,8 @@
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" t="s">
-        <v>23</v>
+      <c r="A120" s="5">
+        <v>44360</v>
       </c>
       <c r="B120" s="2">
         <f>서울!B120+경기!B120</f>
@@ -2758,8 +2812,8 @@
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" t="s">
-        <v>26</v>
+      <c r="A121" s="5">
+        <v>44361</v>
       </c>
       <c r="B121" s="2">
         <f>서울!B121+경기!B121</f>
@@ -2771,8 +2825,8 @@
       </c>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" t="s">
-        <v>27</v>
+      <c r="A122" s="5">
+        <v>44362</v>
       </c>
       <c r="B122" s="2">
         <f>서울!B122+경기!B122</f>
@@ -2784,8 +2838,8 @@
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" t="s">
-        <v>25</v>
+      <c r="A123" s="5">
+        <v>44363</v>
       </c>
       <c r="B123" s="2">
         <f>서울!B123+경기!B123</f>
@@ -2797,8 +2851,8 @@
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" t="s">
-        <v>28</v>
+      <c r="A124" s="5">
+        <v>44364</v>
       </c>
       <c r="B124" s="2">
         <f>서울!B124+경기!B124</f>
@@ -2810,8 +2864,8 @@
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" t="s">
-        <v>29</v>
+      <c r="A125" s="5">
+        <v>44365</v>
       </c>
       <c r="B125" s="2">
         <f>서울!B125+경기!B125</f>
@@ -2823,8 +2877,8 @@
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" t="s">
-        <v>31</v>
+      <c r="A126" s="5">
+        <v>44366</v>
       </c>
       <c r="B126" s="2">
         <f>서울!B126+경기!B126</f>
@@ -2836,8 +2890,8 @@
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" t="s">
-        <v>32</v>
+      <c r="A127" s="5">
+        <v>44367</v>
       </c>
       <c r="B127" s="2">
         <f>서울!B127+경기!B127</f>
@@ -2849,8 +2903,8 @@
       </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" t="s">
-        <v>30</v>
+      <c r="A128" s="5">
+        <v>44368</v>
       </c>
       <c r="B128" s="2">
         <f>서울!B128+경기!B128</f>
@@ -2862,8 +2916,8 @@
       </c>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" t="s">
-        <v>12</v>
+      <c r="A129" s="5">
+        <v>44369</v>
       </c>
       <c r="B129" s="2">
         <f>서울!B129+경기!B129</f>
@@ -2875,8 +2929,8 @@
       </c>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" t="s">
-        <v>13</v>
+      <c r="A130" s="5">
+        <v>44370</v>
       </c>
       <c r="B130" s="2">
         <f>서울!B130+경기!B130</f>
@@ -2888,8 +2942,8 @@
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" t="s">
-        <v>16</v>
+      <c r="A131" s="5">
+        <v>44371</v>
       </c>
       <c r="B131" s="2">
         <f>서울!B131+경기!B131</f>
@@ -2901,8 +2955,8 @@
       </c>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" t="s">
-        <v>14</v>
+      <c r="A132" s="5">
+        <v>44372</v>
       </c>
       <c r="B132" s="2">
         <f>서울!B132+경기!B132</f>
@@ -2914,8 +2968,8 @@
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" t="s">
-        <v>15</v>
+      <c r="A133" s="5">
+        <v>44373</v>
       </c>
       <c r="B133" s="2">
         <f>서울!B133+경기!B133</f>
@@ -2927,8 +2981,8 @@
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" t="s">
-        <v>18</v>
+      <c r="A134" s="5">
+        <v>44374</v>
       </c>
       <c r="B134" s="2">
         <f>서울!B134+경기!B134</f>
@@ -2940,8 +2994,8 @@
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" t="s">
-        <v>19</v>
+      <c r="A135" s="5">
+        <v>44375</v>
       </c>
       <c r="B135" s="2">
         <f>서울!B135+경기!B135</f>
@@ -2953,8 +3007,8 @@
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" t="s">
-        <v>17</v>
+      <c r="A136" s="5">
+        <v>44376</v>
       </c>
       <c r="B136" s="2">
         <f>서울!B136+경기!B136</f>
@@ -2966,8 +3020,8 @@
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" t="s">
-        <v>128</v>
+      <c r="A137" s="5">
+        <v>44377</v>
       </c>
       <c r="B137" s="2">
         <f>서울!B137+경기!B137</f>
@@ -2979,8 +3033,8 @@
       </c>
     </row>
     <row r="138" spans="1:3">
-      <c r="A138" t="s">
-        <v>129</v>
+      <c r="A138" s="5">
+        <v>44378</v>
       </c>
       <c r="B138" s="2">
         <f>서울!B138+경기!B138</f>
@@ -2992,8 +3046,8 @@
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" t="s">
-        <v>131</v>
+      <c r="A139" s="5">
+        <v>44379</v>
       </c>
       <c r="B139" s="2">
         <f>서울!B139+경기!B139</f>
@@ -3005,8 +3059,8 @@
       </c>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" t="s">
-        <v>132</v>
+      <c r="A140" s="5">
+        <v>44380</v>
       </c>
       <c r="B140" s="2">
         <f>서울!B140+경기!B140</f>
@@ -3018,8 +3072,8 @@
       </c>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" t="s">
-        <v>130</v>
+      <c r="A141" s="5">
+        <v>44381</v>
       </c>
       <c r="B141" s="2">
         <f>서울!B141+경기!B141</f>
@@ -3031,8 +3085,8 @@
       </c>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" t="s">
-        <v>134</v>
+      <c r="A142" s="5">
+        <v>44382</v>
       </c>
       <c r="B142" s="2">
         <f>서울!B142+경기!B142</f>
@@ -3044,8 +3098,8 @@
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" t="s">
-        <v>135</v>
+      <c r="A143" s="5">
+        <v>44383</v>
       </c>
       <c r="B143" s="2">
         <f>서울!B143+경기!B143</f>
@@ -3057,8 +3111,8 @@
       </c>
     </row>
     <row r="144" spans="1:3">
-      <c r="A144" t="s">
-        <v>133</v>
+      <c r="A144" s="5">
+        <v>44384</v>
       </c>
       <c r="B144" s="2">
         <f>서울!B144+경기!B144</f>
@@ -3070,8 +3124,8 @@
       </c>
     </row>
     <row r="145" spans="1:3">
-      <c r="A145" t="s">
-        <v>137</v>
+      <c r="A145" s="5">
+        <v>44385</v>
       </c>
       <c r="B145" s="2">
         <f>서울!B145+경기!B145</f>
@@ -3083,8 +3137,8 @@
       </c>
     </row>
     <row r="146" spans="1:3">
-      <c r="A146" t="s">
-        <v>136</v>
+      <c r="A146" s="5">
+        <v>44386</v>
       </c>
       <c r="B146" s="2">
         <f>서울!B146+경기!B146</f>
@@ -3096,8 +3150,8 @@
       </c>
     </row>
     <row r="147" spans="1:3">
-      <c r="A147" t="s">
-        <v>140</v>
+      <c r="A147" s="5">
+        <v>44387</v>
       </c>
       <c r="B147" s="2">
         <f>서울!B147+경기!B147</f>
@@ -3109,8 +3163,8 @@
       </c>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" t="s">
-        <v>139</v>
+      <c r="A148" s="5">
+        <v>44388</v>
       </c>
       <c r="B148" s="2">
         <f>서울!B148+경기!B148</f>
@@ -3122,8 +3176,8 @@
       </c>
     </row>
     <row r="149" spans="1:3">
-      <c r="A149" t="s">
-        <v>138</v>
+      <c r="A149" s="5">
+        <v>44389</v>
       </c>
       <c r="B149" s="2">
         <f>서울!B149+경기!B149</f>
@@ -3135,8 +3189,8 @@
       </c>
     </row>
     <row r="150" spans="1:3">
-      <c r="A150" t="s">
-        <v>142</v>
+      <c r="A150" s="5">
+        <v>44390</v>
       </c>
       <c r="B150" s="2">
         <f>서울!B150+경기!B150</f>
@@ -3148,8 +3202,8 @@
       </c>
     </row>
     <row r="151" spans="1:3">
-      <c r="A151" t="s">
-        <v>143</v>
+      <c r="A151" s="5">
+        <v>44391</v>
       </c>
       <c r="B151" s="2">
         <f>서울!B151+경기!B151</f>
@@ -3161,8 +3215,8 @@
       </c>
     </row>
     <row r="152" spans="1:3">
-      <c r="A152" t="s">
-        <v>141</v>
+      <c r="A152" s="5">
+        <v>44392</v>
       </c>
       <c r="B152" s="2">
         <f>서울!B152+경기!B152</f>
@@ -3174,8 +3228,8 @@
       </c>
     </row>
     <row r="153" spans="1:3">
-      <c r="A153" t="s">
-        <v>144</v>
+      <c r="A153" s="5">
+        <v>44393</v>
       </c>
       <c r="B153" s="2">
         <f>서울!B153+경기!B153</f>
@@ -3187,8 +3241,8 @@
       </c>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" t="s">
-        <v>145</v>
+      <c r="A154" s="5">
+        <v>44394</v>
       </c>
       <c r="B154" s="2">
         <f>서울!B154+경기!B154</f>
@@ -3200,8 +3254,8 @@
       </c>
     </row>
     <row r="155" spans="1:3">
-      <c r="A155" t="s">
-        <v>147</v>
+      <c r="A155" s="5">
+        <v>44395</v>
       </c>
       <c r="B155" s="2">
         <f>서울!B155+경기!B155</f>
@@ -3213,8 +3267,8 @@
       </c>
     </row>
     <row r="156" spans="1:3">
-      <c r="A156" t="s">
-        <v>146</v>
+      <c r="A156" s="5">
+        <v>44396</v>
       </c>
       <c r="B156" s="2">
         <f>서울!B156+경기!B156</f>
@@ -3226,8 +3280,8 @@
       </c>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" t="s">
-        <v>148</v>
+      <c r="A157" s="5">
+        <v>44397</v>
       </c>
       <c r="B157" s="2">
         <f>서울!B157+경기!B157</f>
@@ -3239,8 +3293,8 @@
       </c>
     </row>
     <row r="158" spans="1:3">
-      <c r="A158" t="s">
-        <v>151</v>
+      <c r="A158" s="5">
+        <v>44398</v>
       </c>
       <c r="B158" s="2">
         <f>서울!B158+경기!B158</f>
@@ -3252,8 +3306,8 @@
       </c>
     </row>
     <row r="159" spans="1:3">
-      <c r="A159" t="s">
-        <v>150</v>
+      <c r="A159" s="5">
+        <v>44399</v>
       </c>
       <c r="B159" s="2">
         <f>서울!B159+경기!B159</f>
@@ -3265,8 +3319,8 @@
       </c>
     </row>
     <row r="160" spans="1:3">
-      <c r="A160" t="s">
-        <v>149</v>
+      <c r="A160" s="5">
+        <v>44400</v>
       </c>
       <c r="B160" s="2">
         <f>서울!B160+경기!B160</f>
@@ -3278,8 +3332,8 @@
       </c>
     </row>
     <row r="161" spans="1:3">
-      <c r="A161" t="s">
-        <v>153</v>
+      <c r="A161" s="5">
+        <v>44401</v>
       </c>
       <c r="B161" s="2">
         <f>서울!B161+경기!B161</f>
@@ -3291,8 +3345,8 @@
       </c>
     </row>
     <row r="162" spans="1:3">
-      <c r="A162" t="s">
-        <v>152</v>
+      <c r="A162" s="5">
+        <v>44402</v>
       </c>
       <c r="B162" s="2">
         <f>서울!B162+경기!B162</f>
@@ -3304,8 +3358,8 @@
       </c>
     </row>
     <row r="163" spans="1:3">
-      <c r="A163" t="s">
-        <v>155</v>
+      <c r="A163" s="5">
+        <v>44403</v>
       </c>
       <c r="B163" s="2">
         <f>서울!B163+경기!B163</f>
@@ -3317,8 +3371,8 @@
       </c>
     </row>
     <row r="164" spans="1:3">
-      <c r="A164" t="s">
-        <v>156</v>
+      <c r="A164" s="5">
+        <v>44404</v>
       </c>
       <c r="B164" s="2">
         <f>서울!B164+경기!B164</f>
@@ -3330,8 +3384,8 @@
       </c>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" t="s">
-        <v>154</v>
+      <c r="A165" s="5">
+        <v>44405</v>
       </c>
       <c r="B165" s="2">
         <f>서울!B165+경기!B165</f>
@@ -3343,8 +3397,8 @@
       </c>
     </row>
     <row r="166" spans="1:3">
-      <c r="A166" t="s">
-        <v>157</v>
+      <c r="A166" s="5">
+        <v>44406</v>
       </c>
       <c r="B166" s="2">
         <f>서울!B166+경기!B166</f>
@@ -3356,8 +3410,8 @@
       </c>
     </row>
     <row r="167" spans="1:3">
-      <c r="A167" t="s">
-        <v>159</v>
+      <c r="A167" s="5">
+        <v>44407</v>
       </c>
       <c r="B167" s="2">
         <f>서울!B167+경기!B167</f>
@@ -3369,8 +3423,8 @@
       </c>
     </row>
     <row r="168" spans="1:3">
-      <c r="A168" t="s">
-        <v>158</v>
+      <c r="A168" s="5">
+        <v>44408</v>
       </c>
       <c r="B168" s="2">
         <f>서울!B168+경기!B168</f>
@@ -3382,8 +3436,8 @@
       </c>
     </row>
     <row r="169" spans="1:3">
-      <c r="A169" t="s">
-        <v>160</v>
+      <c r="A169" s="5">
+        <v>44409</v>
       </c>
       <c r="B169" s="2">
         <f>서울!B169+경기!B169</f>
@@ -3395,8 +3449,8 @@
       </c>
     </row>
     <row r="170" spans="1:3">
-      <c r="A170" t="s">
-        <v>161</v>
+      <c r="A170" s="5">
+        <v>44410</v>
       </c>
       <c r="B170" s="2">
         <f>서울!B170+경기!B170</f>
@@ -3408,8 +3462,8 @@
       </c>
     </row>
     <row r="171" spans="1:3">
-      <c r="A171" t="s">
-        <v>163</v>
+      <c r="A171" s="5">
+        <v>44411</v>
       </c>
       <c r="B171" s="2">
         <f>서울!B171+경기!B171</f>
@@ -3421,8 +3475,8 @@
       </c>
     </row>
     <row r="172" spans="1:3">
-      <c r="A172" t="s">
-        <v>162</v>
+      <c r="A172" s="5">
+        <v>44412</v>
       </c>
       <c r="B172" s="2">
         <f>서울!B172+경기!B172</f>
@@ -3434,8 +3488,8 @@
       </c>
     </row>
     <row r="173" spans="1:3">
-      <c r="A173" t="s">
-        <v>164</v>
+      <c r="A173" s="5">
+        <v>44413</v>
       </c>
       <c r="B173" s="2">
         <f>서울!B173+경기!B173</f>
@@ -3447,8 +3501,8 @@
       </c>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" t="s">
-        <v>165</v>
+      <c r="A174" s="5">
+        <v>44414</v>
       </c>
       <c r="B174" s="2">
         <f>서울!B174+경기!B174</f>
@@ -3460,8 +3514,8 @@
       </c>
     </row>
     <row r="175" spans="1:3">
-      <c r="A175" t="s">
-        <v>166</v>
+      <c r="A175" s="5">
+        <v>44415</v>
       </c>
       <c r="B175" s="2">
         <f>서울!B175+경기!B175</f>
@@ -3473,8 +3527,8 @@
       </c>
     </row>
     <row r="176" spans="1:3">
-      <c r="A176" t="s">
-        <v>127</v>
+      <c r="A176" s="5">
+        <v>44416</v>
       </c>
       <c r="B176" s="2">
         <f>서울!B176+경기!B176</f>
@@ -3486,8 +3540,8 @@
       </c>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" t="s">
-        <v>126</v>
+      <c r="A177" s="5">
+        <v>44417</v>
       </c>
       <c r="B177" s="2">
         <f>서울!B177+경기!B177</f>
@@ -3499,8 +3553,8 @@
       </c>
     </row>
     <row r="178" spans="1:3">
-      <c r="A178" t="s">
-        <v>125</v>
+      <c r="A178" s="5">
+        <v>44418</v>
       </c>
       <c r="B178" s="2">
         <f>서울!B178+경기!B178</f>
@@ -3512,8 +3566,8 @@
       </c>
     </row>
     <row r="179" spans="1:3">
-      <c r="A179" t="s">
-        <v>167</v>
+      <c r="A179" s="5">
+        <v>44419</v>
       </c>
       <c r="B179" s="2">
         <f>서울!B179+경기!B179</f>
@@ -3525,8 +3579,8 @@
       </c>
     </row>
     <row r="180" spans="1:3">
-      <c r="A180" t="s">
-        <v>168</v>
+      <c r="A180" s="5">
+        <v>44420</v>
       </c>
       <c r="B180" s="2">
         <f>서울!B180+경기!B180</f>
@@ -3538,8 +3592,8 @@
       </c>
     </row>
     <row r="181" spans="1:3">
-      <c r="A181" t="s">
-        <v>169</v>
+      <c r="A181" s="5">
+        <v>44421</v>
       </c>
       <c r="B181" s="2">
         <f>서울!B181+경기!B181</f>
@@ -3551,8 +3605,8 @@
       </c>
     </row>
     <row r="182" spans="1:3">
-      <c r="A182" t="s">
-        <v>170</v>
+      <c r="A182" s="5">
+        <v>44422</v>
       </c>
       <c r="B182" s="2">
         <f>서울!B182+경기!B182</f>
@@ -3564,8 +3618,8 @@
       </c>
     </row>
     <row r="183" spans="1:3">
-      <c r="A183" t="s">
-        <v>171</v>
+      <c r="A183" s="5">
+        <v>44423</v>
       </c>
       <c r="B183" s="2">
         <f>서울!B183+경기!B183</f>
@@ -3577,8 +3631,8 @@
       </c>
     </row>
     <row r="184" spans="1:3">
-      <c r="A184" t="s">
-        <v>173</v>
+      <c r="A184" s="5">
+        <v>44424</v>
       </c>
       <c r="B184" s="2">
         <f>서울!B184+경기!B184</f>
@@ -3590,8 +3644,8 @@
       </c>
     </row>
     <row r="185" spans="1:3">
-      <c r="A185" t="s">
-        <v>174</v>
+      <c r="A185" s="5">
+        <v>44425</v>
       </c>
       <c r="B185" s="2">
         <f>서울!B185+경기!B185</f>
@@ -3603,8 +3657,8 @@
       </c>
     </row>
     <row r="186" spans="1:3">
-      <c r="A186" t="s">
-        <v>172</v>
+      <c r="A186" s="5">
+        <v>44426</v>
       </c>
       <c r="B186" s="2">
         <f>서울!B186+경기!B186</f>
@@ -3616,8 +3670,8 @@
       </c>
     </row>
     <row r="187" spans="1:3">
-      <c r="A187" t="s">
-        <v>175</v>
+      <c r="A187" s="5">
+        <v>44427</v>
       </c>
       <c r="B187" s="2">
         <f>서울!B187+경기!B187</f>
@@ -3629,8 +3683,8 @@
       </c>
     </row>
     <row r="188" spans="1:3">
-      <c r="A188" t="s">
-        <v>176</v>
+      <c r="A188" s="5">
+        <v>44428</v>
       </c>
       <c r="B188" s="2">
         <f>서울!B188+경기!B188</f>
@@ -3642,8 +3696,8 @@
       </c>
     </row>
     <row r="189" spans="1:3">
-      <c r="A189" t="s">
-        <v>179</v>
+      <c r="A189" s="5">
+        <v>44429</v>
       </c>
       <c r="B189" s="2">
         <f>서울!B189+경기!B189</f>
@@ -3655,8 +3709,8 @@
       </c>
     </row>
     <row r="190" spans="1:3">
-      <c r="A190" t="s">
-        <v>177</v>
+      <c r="A190" s="5">
+        <v>44430</v>
       </c>
       <c r="B190" s="2">
         <f>서울!B190+경기!B190</f>
@@ -3668,8 +3722,8 @@
       </c>
     </row>
     <row r="191" spans="1:3">
-      <c r="A191" t="s">
-        <v>178</v>
+      <c r="A191" s="5">
+        <v>44431</v>
       </c>
       <c r="B191" s="2">
         <f>서울!B191+경기!B191</f>
@@ -3681,8 +3735,8 @@
       </c>
     </row>
     <row r="192" spans="1:3">
-      <c r="A192" t="s">
-        <v>180</v>
+      <c r="A192" s="5">
+        <v>44432</v>
       </c>
       <c r="B192" s="2">
         <f>서울!B192+경기!B192</f>
@@ -3694,8 +3748,8 @@
       </c>
     </row>
     <row r="193" spans="1:3">
-      <c r="A193" t="s">
-        <v>181</v>
+      <c r="A193" s="5">
+        <v>44433</v>
       </c>
       <c r="B193" s="2">
         <f>서울!B193+경기!B193</f>
@@ -3707,8 +3761,8 @@
       </c>
     </row>
     <row r="194" spans="1:3">
-      <c r="A194" t="s">
-        <v>182</v>
+      <c r="A194" s="5">
+        <v>44434</v>
       </c>
       <c r="B194" s="2">
         <f>서울!B194+경기!B194</f>
@@ -3720,8 +3774,8 @@
       </c>
     </row>
     <row r="195" spans="1:3">
-      <c r="A195" t="s">
-        <v>183</v>
+      <c r="A195" s="5">
+        <v>44435</v>
       </c>
       <c r="B195" s="2">
         <f>서울!B195+경기!B195</f>
@@ -3733,8 +3787,8 @@
       </c>
     </row>
     <row r="196" spans="1:3">
-      <c r="A196" t="s">
-        <v>185</v>
+      <c r="A196" s="5">
+        <v>44436</v>
       </c>
       <c r="B196" s="2">
         <f>서울!B196+경기!B196</f>
@@ -3746,8 +3800,8 @@
       </c>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" t="s">
-        <v>184</v>
+      <c r="A197" s="5">
+        <v>44437</v>
       </c>
       <c r="B197" s="2">
         <f>서울!B197+경기!B197</f>
@@ -3759,8 +3813,8 @@
       </c>
     </row>
     <row r="198" spans="1:3">
-      <c r="A198" t="s">
-        <v>187</v>
+      <c r="A198" s="5">
+        <v>44438</v>
       </c>
       <c r="B198" s="2">
         <f>서울!B198+경기!B198</f>
@@ -3772,8 +3826,8 @@
       </c>
     </row>
     <row r="199" spans="1:3">
-      <c r="A199" t="s">
-        <v>186</v>
+      <c r="A199" s="5">
+        <v>44439</v>
       </c>
       <c r="B199" s="2">
         <f>서울!B199+경기!B199</f>
@@ -3784,7 +3838,1370 @@
         <v>223331</v>
       </c>
     </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="5">
+        <v>44440</v>
+      </c>
+      <c r="B200" s="2">
+        <f>서울!B200+경기!B200</f>
+        <v>81061</v>
+      </c>
+      <c r="C200" s="2">
+        <f>서울!C200+경기!C200</f>
+        <v>225004</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="5">
+        <v>44441</v>
+      </c>
+      <c r="B201" s="2">
+        <f>서울!B201+경기!B201</f>
+        <v>88842</v>
+      </c>
+      <c r="C201" s="2">
+        <f>서울!C201+경기!C201</f>
+        <v>208641</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="5">
+        <v>44442</v>
+      </c>
+      <c r="B202" s="2">
+        <f>서울!B202+경기!B202</f>
+        <v>107409</v>
+      </c>
+      <c r="C202" s="2">
+        <f>서울!C202+경기!C202</f>
+        <v>295588</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="5">
+        <v>44443</v>
+      </c>
+      <c r="B203" s="2">
+        <f>서울!B203+경기!B203</f>
+        <v>60569</v>
+      </c>
+      <c r="C203" s="2">
+        <f>서울!C203+경기!C203</f>
+        <v>113820</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="5">
+        <v>44444</v>
+      </c>
+      <c r="B204" s="2">
+        <f>서울!B204+경기!B204</f>
+        <v>4942</v>
+      </c>
+      <c r="C204" s="2">
+        <f>서울!C204+경기!C204</f>
+        <v>4663</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="5">
+        <v>44445</v>
+      </c>
+      <c r="B205" s="2">
+        <f>서울!B205+경기!B205</f>
+        <v>332515</v>
+      </c>
+      <c r="C205" s="2">
+        <f>서울!C205+경기!C205</f>
+        <v>279852</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="5">
+        <v>44446</v>
+      </c>
+      <c r="B206" s="2">
+        <f>서울!B206+경기!B206</f>
+        <v>265425</v>
+      </c>
+      <c r="C206" s="2">
+        <f>서울!C206+경기!C206</f>
+        <v>190401</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="5">
+        <v>44447</v>
+      </c>
+      <c r="B207" s="2">
+        <f>서울!B207+경기!B207</f>
+        <v>176549</v>
+      </c>
+      <c r="C207" s="2">
+        <f>서울!C207+경기!C207</f>
+        <v>132000</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="5">
+        <v>44448</v>
+      </c>
+      <c r="B208" s="2">
+        <f>서울!B208+경기!B208</f>
+        <v>211641</v>
+      </c>
+      <c r="C208" s="2">
+        <f>서울!C208+경기!C208</f>
+        <v>121955</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="6">
+        <v>44449</v>
+      </c>
+      <c r="B209" s="2">
+        <f>서울!B209+경기!B209</f>
+        <v>155986.5</v>
+      </c>
+      <c r="C209" s="2">
+        <f>서울!C209+경기!C209</f>
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="6">
+        <v>44450</v>
+      </c>
+      <c r="B210">
+        <v>155986.5</v>
+      </c>
+      <c r="C210">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="6">
+        <v>44451</v>
+      </c>
+      <c r="B211" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C211" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" s="6">
+        <v>44452</v>
+      </c>
+      <c r="B212" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C212" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" s="6">
+        <v>44453</v>
+      </c>
+      <c r="B213" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C213" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" s="6">
+        <v>44454</v>
+      </c>
+      <c r="B214" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C214" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" s="6">
+        <v>44455</v>
+      </c>
+      <c r="B215" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C215" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" s="6">
+        <v>44456</v>
+      </c>
+      <c r="B216" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C216" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" s="6">
+        <v>44457</v>
+      </c>
+      <c r="B217" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C217" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" s="6">
+        <v>44458</v>
+      </c>
+      <c r="B218" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C218" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" s="6">
+        <v>44459</v>
+      </c>
+      <c r="B219" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C219" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" s="6">
+        <v>44460</v>
+      </c>
+      <c r="B220" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C220" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="6">
+        <v>44461</v>
+      </c>
+      <c r="B221" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C221" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" s="6">
+        <v>44462</v>
+      </c>
+      <c r="B222" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C222" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" s="6">
+        <v>44463</v>
+      </c>
+      <c r="B223" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C223" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" s="6">
+        <v>44464</v>
+      </c>
+      <c r="B224" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C224" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" s="6">
+        <v>44465</v>
+      </c>
+      <c r="B225" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C225" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" s="6">
+        <v>44466</v>
+      </c>
+      <c r="B226" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C226" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" s="6">
+        <v>44467</v>
+      </c>
+      <c r="B227" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C227" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" s="6">
+        <v>44468</v>
+      </c>
+      <c r="B228" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C228" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" s="6">
+        <v>44469</v>
+      </c>
+      <c r="B229" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C229" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" s="6">
+        <v>44470</v>
+      </c>
+      <c r="B230" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C230" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="6">
+        <v>44471</v>
+      </c>
+      <c r="B231" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C231" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="6">
+        <v>44472</v>
+      </c>
+      <c r="B232" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C232" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="6">
+        <v>44473</v>
+      </c>
+      <c r="B233" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C233" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="6">
+        <v>44474</v>
+      </c>
+      <c r="B234" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C234" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" s="6">
+        <v>44475</v>
+      </c>
+      <c r="B235" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C235" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" s="6">
+        <v>44476</v>
+      </c>
+      <c r="B236" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C236" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" s="6">
+        <v>44477</v>
+      </c>
+      <c r="B237" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C237" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" s="6">
+        <v>44478</v>
+      </c>
+      <c r="B238" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C238" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="6">
+        <v>44479</v>
+      </c>
+      <c r="B239" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C239" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" s="6">
+        <v>44480</v>
+      </c>
+      <c r="B240" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C240" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" s="6">
+        <v>44481</v>
+      </c>
+      <c r="B241" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C241" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" s="6">
+        <v>44482</v>
+      </c>
+      <c r="B242" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C242" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" s="6">
+        <v>44483</v>
+      </c>
+      <c r="B243" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C243" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" s="6">
+        <v>44484</v>
+      </c>
+      <c r="B244" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C244" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" s="6">
+        <v>44485</v>
+      </c>
+      <c r="B245" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C245" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" s="6">
+        <v>44486</v>
+      </c>
+      <c r="B246" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C246" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" s="6">
+        <v>44487</v>
+      </c>
+      <c r="B247" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C247" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="6">
+        <v>44488</v>
+      </c>
+      <c r="B248" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C248" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" s="6">
+        <v>44489</v>
+      </c>
+      <c r="B249" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C249" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" s="6">
+        <v>44490</v>
+      </c>
+      <c r="B250" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C250" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" s="6">
+        <v>44491</v>
+      </c>
+      <c r="B251" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C251" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" s="6">
+        <v>44492</v>
+      </c>
+      <c r="B252" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C252" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" s="6">
+        <v>44493</v>
+      </c>
+      <c r="B253" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C253" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" s="6">
+        <v>44494</v>
+      </c>
+      <c r="B254" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C254" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" s="6">
+        <v>44495</v>
+      </c>
+      <c r="B255" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C255" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" s="6">
+        <v>44496</v>
+      </c>
+      <c r="B256" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C256" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" s="6">
+        <v>44497</v>
+      </c>
+      <c r="B257" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C257" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" s="6">
+        <v>44498</v>
+      </c>
+      <c r="B258" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C258" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" s="6">
+        <v>44499</v>
+      </c>
+      <c r="B259" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C259" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="6">
+        <v>44500</v>
+      </c>
+      <c r="B260" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C260" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" s="6">
+        <v>44501</v>
+      </c>
+      <c r="B261" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C261" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" s="6">
+        <v>44502</v>
+      </c>
+      <c r="B262" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C262" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" s="6">
+        <v>44503</v>
+      </c>
+      <c r="B263" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C263" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" s="6">
+        <v>44504</v>
+      </c>
+      <c r="B264" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C264" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265" s="6">
+        <v>44505</v>
+      </c>
+      <c r="B265" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C265" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" s="6">
+        <v>44506</v>
+      </c>
+      <c r="B266" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C266" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" s="6">
+        <v>44507</v>
+      </c>
+      <c r="B267" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C267" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" s="6">
+        <v>44508</v>
+      </c>
+      <c r="B268" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C268" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" s="6">
+        <v>44509</v>
+      </c>
+      <c r="B269" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C269" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" s="6">
+        <v>44510</v>
+      </c>
+      <c r="B270" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C270" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" s="6">
+        <v>44511</v>
+      </c>
+      <c r="B271" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C271" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" s="6">
+        <v>44512</v>
+      </c>
+      <c r="B272" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C272" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" s="6">
+        <v>44513</v>
+      </c>
+      <c r="B273" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C273" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" s="6">
+        <v>44514</v>
+      </c>
+      <c r="B274" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C274" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" s="6">
+        <v>44515</v>
+      </c>
+      <c r="B275" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C275" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" s="6">
+        <v>44516</v>
+      </c>
+      <c r="B276" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C276" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" s="6">
+        <v>44517</v>
+      </c>
+      <c r="B277" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C277" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" s="6">
+        <v>44518</v>
+      </c>
+      <c r="B278" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C278" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" s="6">
+        <v>44519</v>
+      </c>
+      <c r="B279" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C279" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" s="6">
+        <v>44520</v>
+      </c>
+      <c r="B280" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C280" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" s="6">
+        <v>44521</v>
+      </c>
+      <c r="B281" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C281" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" s="6">
+        <v>44522</v>
+      </c>
+      <c r="B282" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C282" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" s="6">
+        <v>44523</v>
+      </c>
+      <c r="B283" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C283" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" s="6">
+        <v>44524</v>
+      </c>
+      <c r="B284" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C284" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" s="6">
+        <v>44525</v>
+      </c>
+      <c r="B285" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C285" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" s="6">
+        <v>44526</v>
+      </c>
+      <c r="B286" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C286" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" s="6">
+        <v>44527</v>
+      </c>
+      <c r="B287" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C287" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" s="6">
+        <v>44528</v>
+      </c>
+      <c r="B288" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C288" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" s="6">
+        <v>44529</v>
+      </c>
+      <c r="B289" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C289" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" s="6">
+        <v>44530</v>
+      </c>
+      <c r="B290" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C290" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" s="6">
+        <v>44531</v>
+      </c>
+      <c r="B291" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C291" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" s="6">
+        <v>44532</v>
+      </c>
+      <c r="B292" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C292" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" s="6">
+        <v>44533</v>
+      </c>
+      <c r="B293" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C293" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
+      <c r="A294" s="6">
+        <v>44534</v>
+      </c>
+      <c r="B294" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C294" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" s="6">
+        <v>44535</v>
+      </c>
+      <c r="B295" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C295" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" s="6">
+        <v>44536</v>
+      </c>
+      <c r="B296" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C296" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" s="6">
+        <v>44537</v>
+      </c>
+      <c r="B297" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C297" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" s="6">
+        <v>44538</v>
+      </c>
+      <c r="B298" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C298" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="A299" s="6">
+        <v>44539</v>
+      </c>
+      <c r="B299" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C299" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3">
+      <c r="A300" s="6">
+        <v>44540</v>
+      </c>
+      <c r="B300" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C300" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="A301" s="6">
+        <v>44541</v>
+      </c>
+      <c r="B301" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C301" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="A302" s="6">
+        <v>44542</v>
+      </c>
+      <c r="B302" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C302" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="A303" s="6">
+        <v>44543</v>
+      </c>
+      <c r="B303" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C303" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3">
+      <c r="A304" s="6">
+        <v>44544</v>
+      </c>
+      <c r="B304" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C304" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3">
+      <c r="A305" s="6">
+        <v>44545</v>
+      </c>
+      <c r="B305" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C305" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3">
+      <c r="A306" s="6">
+        <v>44546</v>
+      </c>
+      <c r="B306" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C306" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3">
+      <c r="A307" s="6">
+        <v>44547</v>
+      </c>
+      <c r="B307" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C307" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3">
+      <c r="A308" s="6">
+        <v>44548</v>
+      </c>
+      <c r="B308" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C308" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3">
+      <c r="A309" s="6">
+        <v>44549</v>
+      </c>
+      <c r="B309" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C309" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3">
+      <c r="A310" s="6">
+        <v>44550</v>
+      </c>
+      <c r="B310" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C310" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3">
+      <c r="A311" s="6">
+        <v>44551</v>
+      </c>
+      <c r="B311" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C311" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3">
+      <c r="A312" s="6">
+        <v>44552</v>
+      </c>
+      <c r="B312" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C312" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3">
+      <c r="A313" s="6">
+        <v>44553</v>
+      </c>
+      <c r="B313" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C313" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3">
+      <c r="A314" s="6">
+        <v>44554</v>
+      </c>
+      <c r="B314" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C314" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3">
+      <c r="A315" s="6">
+        <v>44555</v>
+      </c>
+      <c r="B315" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C315" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3">
+      <c r="A316" s="6">
+        <v>44556</v>
+      </c>
+      <c r="B316" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C316" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3">
+      <c r="A317" s="6">
+        <v>44557</v>
+      </c>
+      <c r="B317" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C317" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3">
+      <c r="A318" s="6">
+        <v>44558</v>
+      </c>
+      <c r="B318" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C318" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3">
+      <c r="A319" s="6">
+        <v>44559</v>
+      </c>
+      <c r="B319" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C319" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3">
+      <c r="A320" s="6">
+        <v>44560</v>
+      </c>
+      <c r="B320" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C320" s="1">
+        <v>168365</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3">
+      <c r="A321" s="6">
+        <v>44561</v>
+      </c>
+      <c r="B321" s="1">
+        <v>155986.5</v>
+      </c>
+      <c r="C321" s="1">
+        <v>168365</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
 </worksheet>
@@ -3793,10 +5210,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C209"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A195" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="B209" sqref="B209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -5993,7 +7410,120 @@
         <v>95981</v>
       </c>
     </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B200" s="2">
+        <v>34235</v>
+      </c>
+      <c r="C200" s="2">
+        <v>94420</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B201" s="2">
+        <v>39320</v>
+      </c>
+      <c r="C201" s="2">
+        <v>88297</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B202" s="2">
+        <v>45045</v>
+      </c>
+      <c r="C202" s="2">
+        <v>113133</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B203" s="2">
+        <v>22326</v>
+      </c>
+      <c r="C203" s="2">
+        <v>42787</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B204" s="2">
+        <v>1388</v>
+      </c>
+      <c r="C204" s="2">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205" s="2">
+        <v>145248</v>
+      </c>
+      <c r="C205" s="2">
+        <v>116054</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B206" s="2">
+        <v>111410</v>
+      </c>
+      <c r="C206" s="2">
+        <v>80167</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B207" s="2">
+        <v>73677</v>
+      </c>
+      <c r="C207" s="2">
+        <v>54596</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B208" s="2">
+        <v>91416</v>
+      </c>
+      <c r="C208" s="2">
+        <v>50641</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B209" s="2">
+        <f>AVERAGE(B201:B208)</f>
+        <v>66228.75</v>
+      </c>
+      <c r="C209" s="2">
+        <f>AVERAGE(C201:C208)</f>
+        <v>68406.875</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
 </worksheet>
@@ -6002,10 +7532,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A192" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="D213" sqref="D213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -8202,8 +9732,121 @@
         <v>127350</v>
       </c>
     </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B200" s="1">
+        <v>46826</v>
+      </c>
+      <c r="C200" s="1">
+        <v>130584</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B201" s="1">
+        <v>49522</v>
+      </c>
+      <c r="C201" s="1">
+        <v>120344</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B202" s="1">
+        <v>62364</v>
+      </c>
+      <c r="C202" s="1">
+        <v>182455</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B203" s="1">
+        <v>38243</v>
+      </c>
+      <c r="C203" s="1">
+        <v>71033</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B204" s="1">
+        <v>3554</v>
+      </c>
+      <c r="C204" s="1">
+        <v>3083</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205" s="1">
+        <v>187267</v>
+      </c>
+      <c r="C205" s="1">
+        <v>163798</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B206" s="1">
+        <v>154015</v>
+      </c>
+      <c r="C206" s="1">
+        <v>110234</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B207" s="1">
+        <v>102872</v>
+      </c>
+      <c r="C207" s="1">
+        <v>77404</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B208" s="1">
+        <v>120225</v>
+      </c>
+      <c r="C208" s="1">
+        <v>71314</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B209" s="2">
+        <f>AVERAGE(B201:B208)</f>
+        <v>89757.75</v>
+      </c>
+      <c r="C209" s="2">
+        <f>AVERAGE(C201:C208)</f>
+        <v>99958.125</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change daily vaccination number
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccination_number.xlsx
+++ b/data/vaccine/vaccination_number.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyunjeong/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE330C6-2F28-1245-870C-2322D6028C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1745AC08-8966-354C-B858-FCED3157C399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23260" yWindow="1680" windowWidth="13180" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="20920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total" sheetId="1" r:id="rId1"/>
@@ -1247,8 +1247,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="D320" sqref="D320"/>
+    <sheetView tabSelected="1" topLeftCell="A298" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="C210" sqref="C210:C321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -3960,7 +3960,6 @@
         <v>44449</v>
       </c>
       <c r="B209" s="2">
-        <f>서울!B209+경기!B209</f>
         <v>155986.5</v>
       </c>
       <c r="C209" s="2">
@@ -3972,1456 +3971,1232 @@
       <c r="A210" s="6">
         <v>44450</v>
       </c>
-      <c r="B210">
-        <f>$B$209/3</f>
-        <v>51995.5</v>
+      <c r="B210" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C210">
-        <f>$C$209/2</f>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="6">
         <v>44451</v>
       </c>
-      <c r="B211" s="1">
-        <f t="shared" ref="B211:B274" si="0">$B$209/3</f>
-        <v>51995.5</v>
+      <c r="B211" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C211" s="1">
-        <f t="shared" ref="C211:C274" si="1">$C$209/2</f>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="6">
         <v>44452</v>
       </c>
-      <c r="B212" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B212" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C212" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="6">
         <v>44453</v>
       </c>
-      <c r="B213" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B213" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C213" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" s="6">
         <v>44454</v>
       </c>
-      <c r="B214" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B214" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C214" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" s="6">
         <v>44455</v>
       </c>
-      <c r="B215" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B215" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C215" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="6">
         <v>44456</v>
       </c>
-      <c r="B216" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B216" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C216" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="6">
         <v>44457</v>
       </c>
-      <c r="B217" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B217" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C217" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="6">
         <v>44458</v>
       </c>
-      <c r="B218" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B218" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C218" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" s="6">
         <v>44459</v>
       </c>
-      <c r="B219" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B219" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C219" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" s="6">
         <v>44460</v>
       </c>
-      <c r="B220" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B220" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C220" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="6">
         <v>44461</v>
       </c>
-      <c r="B221" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B221" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C221" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="6">
         <v>44462</v>
       </c>
-      <c r="B222" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B222" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C222" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" s="6">
         <v>44463</v>
       </c>
-      <c r="B223" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B223" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C223" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" s="6">
         <v>44464</v>
       </c>
-      <c r="B224" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B224" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C224" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="6">
         <v>44465</v>
       </c>
-      <c r="B225" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B225" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C225" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="6">
         <v>44466</v>
       </c>
-      <c r="B226" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B226" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C226" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" s="6">
         <v>44467</v>
       </c>
-      <c r="B227" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B227" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C227" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="6">
         <v>44468</v>
       </c>
-      <c r="B228" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B228" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C228" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" s="6">
         <v>44469</v>
       </c>
-      <c r="B229" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B229" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C229" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="6">
         <v>44470</v>
       </c>
-      <c r="B230" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B230" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C230" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="6">
         <v>44471</v>
       </c>
-      <c r="B231" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B231" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C231" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="6">
         <v>44472</v>
       </c>
-      <c r="B232" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B232" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C232" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="6">
         <v>44473</v>
       </c>
-      <c r="B233" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B233" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C233" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="6">
         <v>44474</v>
       </c>
-      <c r="B234" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B234" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C234" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="6">
         <v>44475</v>
       </c>
-      <c r="B235" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B235" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C235" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="6">
         <v>44476</v>
       </c>
-      <c r="B236" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B236" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C236" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="6">
         <v>44477</v>
       </c>
-      <c r="B237" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B237" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C237" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="6">
         <v>44478</v>
       </c>
-      <c r="B238" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B238" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C238" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" s="6">
         <v>44479</v>
       </c>
-      <c r="B239" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B239" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C239" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" s="6">
         <v>44480</v>
       </c>
-      <c r="B240" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B240" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C240" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" s="6">
         <v>44481</v>
       </c>
-      <c r="B241" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B241" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C241" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="6">
         <v>44482</v>
       </c>
-      <c r="B242" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B242" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C242" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" s="6">
         <v>44483</v>
       </c>
-      <c r="B243" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B243" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C243" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="6">
         <v>44484</v>
       </c>
-      <c r="B244" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B244" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C244" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="6">
         <v>44485</v>
       </c>
-      <c r="B245" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B245" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C245" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="6">
         <v>44486</v>
       </c>
-      <c r="B246" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B246" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C246" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="6">
         <v>44487</v>
       </c>
-      <c r="B247" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B247" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C247" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="6">
         <v>44488</v>
       </c>
-      <c r="B248" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B248" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C248" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="6">
         <v>44489</v>
       </c>
-      <c r="B249" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B249" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C249" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" s="6">
         <v>44490</v>
       </c>
-      <c r="B250" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B250" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C250" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" s="6">
         <v>44491</v>
       </c>
-      <c r="B251" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B251" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C251" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="6">
         <v>44492</v>
       </c>
-      <c r="B252" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B252" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C252" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" s="6">
         <v>44493</v>
       </c>
-      <c r="B253" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B253" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C253" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254" s="6">
         <v>44494</v>
       </c>
-      <c r="B254" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B254" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C254" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" s="6">
         <v>44495</v>
       </c>
-      <c r="B255" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B255" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C255" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="6">
         <v>44496</v>
       </c>
-      <c r="B256" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B256" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C256" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" s="6">
         <v>44497</v>
       </c>
-      <c r="B257" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B257" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C257" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" s="6">
         <v>44498</v>
       </c>
-      <c r="B258" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B258" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C258" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" s="6">
         <v>44499</v>
       </c>
-      <c r="B259" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B259" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C259" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="6">
         <v>44500</v>
       </c>
-      <c r="B260" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B260" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C260" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" s="6">
         <v>44501</v>
       </c>
-      <c r="B261" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B261" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C261" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" s="6">
         <v>44502</v>
       </c>
-      <c r="B262" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B262" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C262" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" s="6">
         <v>44503</v>
       </c>
-      <c r="B263" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B263" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C263" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="6">
         <v>44504</v>
       </c>
-      <c r="B264" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B264" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C264" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" s="6">
         <v>44505</v>
       </c>
-      <c r="B265" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B265" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C265" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" s="6">
         <v>44506</v>
       </c>
-      <c r="B266" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B266" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C266" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" s="6">
         <v>44507</v>
       </c>
-      <c r="B267" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B267" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C267" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" s="6">
         <v>44508</v>
       </c>
-      <c r="B268" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B268" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C268" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" s="6">
         <v>44509</v>
       </c>
-      <c r="B269" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B269" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C269" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" s="6">
         <v>44510</v>
       </c>
-      <c r="B270" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B270" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C270" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="6">
         <v>44511</v>
       </c>
-      <c r="B271" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B271" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C271" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="6">
         <v>44512</v>
       </c>
-      <c r="B272" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B272" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C272" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" s="6">
         <v>44513</v>
       </c>
-      <c r="B273" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B273" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C273" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="274" spans="1:3">
       <c r="A274" s="6">
         <v>44514</v>
       </c>
-      <c r="B274" s="1">
-        <f t="shared" si="0"/>
-        <v>51995.5</v>
+      <c r="B274" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C274" s="1">
-        <f t="shared" si="1"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="275" spans="1:3">
       <c r="A275" s="6">
         <v>44515</v>
       </c>
-      <c r="B275" s="1">
-        <f t="shared" ref="B275:B321" si="2">$B$209/3</f>
-        <v>51995.5</v>
+      <c r="B275" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C275" s="1">
-        <f t="shared" ref="C275:C321" si="3">$C$209/2</f>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" s="6">
         <v>44516</v>
       </c>
-      <c r="B276" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B276" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C276" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="277" spans="1:3">
       <c r="A277" s="6">
         <v>44517</v>
       </c>
-      <c r="B277" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B277" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C277" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="278" spans="1:3">
       <c r="A278" s="6">
         <v>44518</v>
       </c>
-      <c r="B278" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B278" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C278" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" s="6">
         <v>44519</v>
       </c>
-      <c r="B279" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B279" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C279" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="280" spans="1:3">
       <c r="A280" s="6">
         <v>44520</v>
       </c>
-      <c r="B280" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B280" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C280" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" s="6">
         <v>44521</v>
       </c>
-      <c r="B281" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B281" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C281" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" s="6">
         <v>44522</v>
       </c>
-      <c r="B282" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B282" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C282" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="6">
         <v>44523</v>
       </c>
-      <c r="B283" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B283" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C283" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" s="6">
         <v>44524</v>
       </c>
-      <c r="B284" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B284" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C284" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" s="6">
         <v>44525</v>
       </c>
-      <c r="B285" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B285" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C285" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" s="6">
         <v>44526</v>
       </c>
-      <c r="B286" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B286" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C286" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="287" spans="1:3">
       <c r="A287" s="6">
         <v>44527</v>
       </c>
-      <c r="B287" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B287" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C287" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="288" spans="1:3">
       <c r="A288" s="6">
         <v>44528</v>
       </c>
-      <c r="B288" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B288" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C288" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="289" spans="1:3">
       <c r="A289" s="6">
         <v>44529</v>
       </c>
-      <c r="B289" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B289" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C289" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="290" spans="1:3">
       <c r="A290" s="6">
         <v>44530</v>
       </c>
-      <c r="B290" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B290" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C290" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" s="6">
         <v>44531</v>
       </c>
-      <c r="B291" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B291" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C291" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="292" spans="1:3">
       <c r="A292" s="6">
         <v>44532</v>
       </c>
-      <c r="B292" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B292" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C292" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="A293" s="6">
         <v>44533</v>
       </c>
-      <c r="B293" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B293" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C293" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" s="6">
         <v>44534</v>
       </c>
-      <c r="B294" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B294" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C294" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="295" spans="1:3">
       <c r="A295" s="6">
         <v>44535</v>
       </c>
-      <c r="B295" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B295" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C295" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="296" spans="1:3">
       <c r="A296" s="6">
         <v>44536</v>
       </c>
-      <c r="B296" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B296" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C296" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="297" spans="1:3">
       <c r="A297" s="6">
         <v>44537</v>
       </c>
-      <c r="B297" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B297" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C297" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="6">
         <v>44538</v>
       </c>
-      <c r="B298" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B298" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C298" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="299" spans="1:3">
       <c r="A299" s="6">
         <v>44539</v>
       </c>
-      <c r="B299" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B299" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C299" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="300" spans="1:3">
       <c r="A300" s="6">
         <v>44540</v>
       </c>
-      <c r="B300" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B300" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C300" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="301" spans="1:3">
       <c r="A301" s="6">
         <v>44541</v>
       </c>
-      <c r="B301" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B301" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C301" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" s="6">
         <v>44542</v>
       </c>
-      <c r="B302" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B302" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C302" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="303" spans="1:3">
       <c r="A303" s="6">
         <v>44543</v>
       </c>
-      <c r="B303" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B303" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C303" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="304" spans="1:3">
       <c r="A304" s="6">
         <v>44544</v>
       </c>
-      <c r="B304" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B304" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C304" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="305" spans="1:3">
       <c r="A305" s="6">
         <v>44545</v>
       </c>
-      <c r="B305" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B305" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C305" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="306" spans="1:3">
       <c r="A306" s="6">
         <v>44546</v>
       </c>
-      <c r="B306" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B306" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C306" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="307" spans="1:3">
       <c r="A307" s="6">
         <v>44547</v>
       </c>
-      <c r="B307" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B307" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C307" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="308" spans="1:3">
       <c r="A308" s="6">
         <v>44548</v>
       </c>
-      <c r="B308" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B308" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C308" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="309" spans="1:3">
       <c r="A309" s="6">
         <v>44549</v>
       </c>
-      <c r="B309" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B309" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C309" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="310" spans="1:3">
       <c r="A310" s="6">
         <v>44550</v>
       </c>
-      <c r="B310" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B310" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C310" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="311" spans="1:3">
       <c r="A311" s="6">
         <v>44551</v>
       </c>
-      <c r="B311" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B311" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C311" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="312" spans="1:3">
       <c r="A312" s="6">
         <v>44552</v>
       </c>
-      <c r="B312" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B312" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C312" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="6">
         <v>44553</v>
       </c>
-      <c r="B313" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B313" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C313" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="314" spans="1:3">
       <c r="A314" s="6">
         <v>44554</v>
       </c>
-      <c r="B314" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B314" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C314" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="315" spans="1:3">
       <c r="A315" s="6">
         <v>44555</v>
       </c>
-      <c r="B315" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B315" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C315" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="316" spans="1:3">
       <c r="A316" s="6">
         <v>44556</v>
       </c>
-      <c r="B316" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B316" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C316" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="317" spans="1:3">
       <c r="A317" s="6">
         <v>44557</v>
       </c>
-      <c r="B317" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B317" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C317" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="318" spans="1:3">
       <c r="A318" s="6">
         <v>44558</v>
       </c>
-      <c r="B318" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B318" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C318" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="319" spans="1:3">
       <c r="A319" s="6">
         <v>44559</v>
       </c>
-      <c r="B319" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B319" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C319" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="6">
         <v>44560</v>
       </c>
-      <c r="B320" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B320" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C320" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
     <row r="321" spans="1:3">
       <c r="A321" s="6">
         <v>44561</v>
       </c>
-      <c r="B321" s="1">
-        <f t="shared" si="2"/>
-        <v>51995.5</v>
+      <c r="B321" s="2">
+        <v>155986.5</v>
       </c>
       <c r="C321" s="1">
-        <f t="shared" si="3"/>
-        <v>84182.5</v>
+        <v>168365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>